<commit_message>
added backtesting and golden cross
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Melvin\Project\Python\stk_advisor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\python\git_repo\stk_advisor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6090FE-9B80-4062-B2A8-4F558E76FB7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1772511-2EF0-4545-AB28-5D0395A0CED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13980" yWindow="375" windowWidth="13335" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3570" yWindow="960" windowWidth="25935" windowHeight="18885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="portfolio" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Symbol</t>
   </si>
@@ -90,18 +90,6 @@
   </si>
   <si>
     <t>Total Stock,International</t>
-  </si>
-  <si>
-    <t>JEPI</t>
-  </si>
-  <si>
-    <t>PEY</t>
-  </si>
-  <si>
-    <t>SPYD</t>
-  </si>
-  <si>
-    <t>FAS</t>
   </si>
 </sst>
 </file>
@@ -951,10 +939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,26 +1037,6 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added tax implication logic
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\python\git_repo\stk_advisor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04ABB338-98E9-42E1-9D0C-18773E6853D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79C4845-2FE0-48E9-86FE-BB9600045665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="portfolio" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
   <si>
     <t>Symbol</t>
   </si>
@@ -122,19 +122,44 @@
     <t>QQQ</t>
   </si>
   <si>
-    <t>PURCHASE  DATE</t>
-  </si>
-  <si>
-    <t>PURCHASE PRICE</t>
-  </si>
-  <si>
-    <t>PURCHASE QTY</t>
+    <t>PURCHASE _DATE</t>
+  </si>
+  <si>
+    <t>PURCHASE_PRICE</t>
+  </si>
+  <si>
+    <t>PURCHASE_QTY</t>
+  </si>
+  <si>
+    <t>2024-04-09</t>
+  </si>
+  <si>
+    <t>2022-07-28</t>
+  </si>
+  <si>
+    <t>2024-04-03</t>
+  </si>
+  <si>
+    <t>2024-01-03</t>
+  </si>
+  <si>
+    <t>2024-04-02</t>
+  </si>
+  <si>
+    <t>2024-03-12</t>
+  </si>
+  <si>
+    <t>2024-03-06</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -574,7 +599,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -617,14 +642,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
@@ -652,6 +686,7 @@
     <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Currency" xfId="42" builtinId="4"/>
     <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="29" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="30" builtinId="16" customBuiltin="1"/>
@@ -978,10 +1013,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,12 +1024,12 @@
     <col min="1" max="1" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1014,7 +1049,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -1024,10 +1059,18 @@
       <c r="C2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="2">
+        <v>106.71</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -1037,8 +1080,18 @@
       <c r="C3" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="2">
+        <v>53.56</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1048,8 +1101,18 @@
       <c r="C4" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="2">
+        <v>79.73</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1059,8 +1122,18 @@
       <c r="C5" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="2">
+        <v>86.67</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1070,8 +1143,18 @@
       <c r="C6" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="2">
+        <v>256.83999999999997</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -1081,8 +1164,18 @@
       <c r="C7" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="2">
+        <v>60</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -1092,8 +1185,18 @@
       <c r="C8" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="2">
+        <v>41.65</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -1103,8 +1206,18 @@
       <c r="C9" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="2">
+        <v>206.81</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -1112,34 +1225,50 @@
         <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="1"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="1"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -1149,8 +1278,12 @@
       <c r="C14" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="1"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -1160,6 +1293,18 @@
       <c r="C15" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="3"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C15">

</xml_diff>